<commit_message>
Fix some augment and slavers affix types
</commit_message>
<xml_diff>
--- a/data-builder/slavers.xlsx
+++ b/data-builder/slavers.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9672" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9675" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Prefix" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="Bonus" sheetId="4" r:id="rId4"/>
     <sheet name="Set" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="81">
   <si>
     <t>Strength</t>
   </si>
@@ -263,12 +263,15 @@
   </si>
   <si>
     <t>Spell Saves</t>
+  </si>
+  <si>
+    <t>Competence</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -607,7 +610,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -618,15 +621,15 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A9"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.42578125" customWidth="1"/>
+    <col min="2" max="2" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -932,11 +935,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27:B51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -963,7 +969,7 @@
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -991,7 +997,7 @@
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -1313,7 +1319,7 @@
         <v>28</v>
       </c>
       <c r="D27" t="s">
-        <v>14</v>
+        <v>80</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -1341,10 +1347,10 @@
         <v>14</v>
       </c>
       <c r="D29" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>18</v>
       </c>
@@ -1358,7 +1364,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>19</v>
       </c>
@@ -1372,7 +1378,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>20</v>
       </c>
@@ -1386,7 +1392,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>21</v>
       </c>
@@ -1400,7 +1406,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>22</v>
       </c>
@@ -1414,7 +1420,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>23</v>
       </c>
@@ -1428,7 +1434,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>24</v>
       </c>
@@ -1442,7 +1448,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>25</v>
       </c>
@@ -1456,7 +1462,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>26</v>
       </c>
@@ -1470,7 +1476,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>27</v>
       </c>
@@ -1484,7 +1490,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>28</v>
       </c>
@@ -1498,7 +1504,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>29</v>
       </c>
@@ -1512,7 +1518,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>30</v>
       </c>
@@ -1526,7 +1532,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>31</v>
       </c>
@@ -1540,7 +1546,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>32</v>
       </c>
@@ -1554,7 +1560,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>33</v>
       </c>
@@ -1568,7 +1574,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>34</v>
       </c>
@@ -1582,7 +1588,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>35</v>
       </c>
@@ -1596,7 +1602,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>36</v>
       </c>
@@ -1610,7 +1616,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>26</v>
       </c>
@@ -1624,7 +1630,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>37</v>
       </c>
@@ -1638,7 +1644,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>38</v>
       </c>
@@ -1662,18 +1668,18 @@
   <dimension ref="A1:D55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A22"/>
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -1687,7 +1693,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -1698,10 +1704,10 @@
         <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -1712,10 +1718,10 @@
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -1726,10 +1732,10 @@
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -1740,10 +1746,10 @@
         <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -1754,10 +1760,10 @@
         <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>45</v>
       </c>
@@ -1768,10 +1774,10 @@
         <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>46</v>
       </c>
@@ -1782,10 +1788,10 @@
         <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>47</v>
       </c>
@@ -1796,10 +1802,10 @@
         <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>48</v>
       </c>
@@ -1810,10 +1816,10 @@
         <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>49</v>
       </c>
@@ -1824,10 +1830,10 @@
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>50</v>
       </c>
@@ -1838,10 +1844,10 @@
         <v>10</v>
       </c>
       <c r="D12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>51</v>
       </c>
@@ -1852,10 +1858,10 @@
         <v>10</v>
       </c>
       <c r="D13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>52</v>
       </c>
@@ -1866,10 +1872,10 @@
         <v>10</v>
       </c>
       <c r="D14" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>53</v>
       </c>
@@ -1880,10 +1886,10 @@
         <v>10</v>
       </c>
       <c r="D15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>54</v>
       </c>
@@ -1894,10 +1900,10 @@
         <v>10</v>
       </c>
       <c r="D16" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>55</v>
       </c>
@@ -1908,10 +1914,10 @@
         <v>10</v>
       </c>
       <c r="D17" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>56</v>
       </c>
@@ -1922,10 +1928,10 @@
         <v>10</v>
       </c>
       <c r="D18" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>57</v>
       </c>
@@ -1936,10 +1942,10 @@
         <v>10</v>
       </c>
       <c r="D19" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>58</v>
       </c>
@@ -1950,10 +1956,10 @@
         <v>10</v>
       </c>
       <c r="D20" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>59</v>
       </c>
@@ -1964,10 +1970,10 @@
         <v>10</v>
       </c>
       <c r="D21" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>60</v>
       </c>
@@ -1978,10 +1984,10 @@
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>61</v>
       </c>
@@ -1995,7 +2001,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>62</v>
       </c>
@@ -2009,7 +2015,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>63</v>
       </c>
@@ -2023,7 +2029,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>65</v>
       </c>
@@ -2037,7 +2043,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>66</v>
       </c>
@@ -2051,7 +2057,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>64</v>
       </c>
@@ -2065,7 +2071,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>40</v>
       </c>
@@ -2076,10 +2082,10 @@
         <v>22</v>
       </c>
       <c r="D29" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>41</v>
       </c>
@@ -2090,10 +2096,10 @@
         <v>22</v>
       </c>
       <c r="D30" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>42</v>
       </c>
@@ -2104,10 +2110,10 @@
         <v>22</v>
       </c>
       <c r="D31" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>43</v>
       </c>
@@ -2118,10 +2124,10 @@
         <v>22</v>
       </c>
       <c r="D32" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>44</v>
       </c>
@@ -2132,10 +2138,10 @@
         <v>22</v>
       </c>
       <c r="D33" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>45</v>
       </c>
@@ -2146,10 +2152,10 @@
         <v>22</v>
       </c>
       <c r="D34" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>46</v>
       </c>
@@ -2160,10 +2166,10 @@
         <v>22</v>
       </c>
       <c r="D35" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>47</v>
       </c>
@@ -2174,10 +2180,10 @@
         <v>22</v>
       </c>
       <c r="D36" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>48</v>
       </c>
@@ -2188,10 +2194,10 @@
         <v>22</v>
       </c>
       <c r="D37" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>49</v>
       </c>
@@ -2202,10 +2208,10 @@
         <v>22</v>
       </c>
       <c r="D38" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>50</v>
       </c>
@@ -2216,10 +2222,10 @@
         <v>22</v>
       </c>
       <c r="D39" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>51</v>
       </c>
@@ -2230,10 +2236,10 @@
         <v>22</v>
       </c>
       <c r="D40" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>52</v>
       </c>
@@ -2244,10 +2250,10 @@
         <v>22</v>
       </c>
       <c r="D41" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>53</v>
       </c>
@@ -2258,10 +2264,10 @@
         <v>22</v>
       </c>
       <c r="D42" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>54</v>
       </c>
@@ -2272,10 +2278,10 @@
         <v>22</v>
       </c>
       <c r="D43" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>55</v>
       </c>
@@ -2286,10 +2292,10 @@
         <v>22</v>
       </c>
       <c r="D44" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>56</v>
       </c>
@@ -2300,10 +2306,10 @@
         <v>22</v>
       </c>
       <c r="D45" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>57</v>
       </c>
@@ -2314,10 +2320,10 @@
         <v>22</v>
       </c>
       <c r="D46" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>58</v>
       </c>
@@ -2328,10 +2334,10 @@
         <v>22</v>
       </c>
       <c r="D47" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>59</v>
       </c>
@@ -2342,10 +2348,10 @@
         <v>22</v>
       </c>
       <c r="D48" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>60</v>
       </c>
@@ -2356,10 +2362,10 @@
         <v>7</v>
       </c>
       <c r="D49" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>61</v>
       </c>
@@ -2373,7 +2379,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>62</v>
       </c>
@@ -2387,7 +2393,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>63</v>
       </c>
@@ -2401,7 +2407,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>65</v>
       </c>
@@ -2415,7 +2421,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>66</v>
       </c>
@@ -2429,7 +2435,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>64</v>
       </c>
@@ -2452,11 +2458,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D61"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -2864,7 +2870,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>58</v>
       </c>
@@ -2878,7 +2884,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>59</v>
       </c>
@@ -2892,7 +2898,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>0</v>
       </c>
@@ -2906,7 +2912,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>2</v>
       </c>
@@ -2920,7 +2926,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>3</v>
       </c>
@@ -2934,7 +2940,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>4</v>
       </c>
@@ -2948,7 +2954,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>5</v>
       </c>
@@ -2962,7 +2968,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>6</v>
       </c>
@@ -2976,7 +2982,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>1</v>
       </c>
@@ -2990,7 +2996,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>7</v>
       </c>
@@ -3004,7 +3010,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>67</v>
       </c>
@@ -3018,7 +3024,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>68</v>
       </c>
@@ -3032,7 +3038,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>40</v>
       </c>
@@ -3046,7 +3052,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>41</v>
       </c>
@@ -3060,7 +3066,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -3074,7 +3080,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>43</v>
       </c>
@@ -3088,7 +3094,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>44</v>
       </c>
@@ -3102,7 +3108,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>45</v>
       </c>
@@ -3116,7 +3122,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>46</v>
       </c>
@@ -3130,7 +3136,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>47</v>
       </c>
@@ -3144,7 +3150,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>48</v>
       </c>
@@ -3158,7 +3164,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>49</v>
       </c>
@@ -3172,7 +3178,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>50</v>
       </c>
@@ -3186,7 +3192,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>51</v>
       </c>
@@ -3200,7 +3206,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>52</v>
       </c>
@@ -3214,7 +3220,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>53</v>
       </c>
@@ -3228,7 +3234,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>54</v>
       </c>
@@ -3242,7 +3248,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>55</v>
       </c>
@@ -3256,7 +3262,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>56</v>
       </c>
@@ -3270,7 +3276,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>57</v>
       </c>
@@ -3284,7 +3290,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>58</v>
       </c>
@@ -3298,7 +3304,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>59</v>
       </c>
@@ -3321,14 +3327,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -3911,7 +3917,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>76</v>
       </c>
@@ -3931,7 +3937,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>76</v>
       </c>
@@ -3951,7 +3957,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>78</v>
       </c>
@@ -3971,7 +3977,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>78</v>
       </c>
@@ -3991,7 +3997,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>78</v>
       </c>
@@ -4011,7 +4017,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>78</v>
       </c>
@@ -4031,7 +4037,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>78</v>
       </c>
@@ -4051,7 +4057,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>78</v>
       </c>
@@ -4071,7 +4077,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>78</v>
       </c>
@@ -4091,7 +4097,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>78</v>
       </c>
@@ -4111,7 +4117,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>78</v>
       </c>
@@ -4131,7 +4137,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>78</v>
       </c>
@@ -4151,7 +4157,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>78</v>
       </c>
@@ -4171,7 +4177,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>78</v>
       </c>
@@ -4191,7 +4197,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>78</v>
       </c>
@@ -4211,7 +4217,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>78</v>
       </c>
@@ -4231,7 +4237,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>78</v>
       </c>
@@ -4251,7 +4257,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>78</v>
       </c>
@@ -4271,7 +4277,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>78</v>
       </c>
@@ -4291,7 +4297,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>78</v>
       </c>

</xml_diff>

<commit_message>
slavers fixes, start synonyms, ml on sets
</commit_message>
<xml_diff>
--- a/data-builder/slavers.xlsx
+++ b/data-builder/slavers.xlsx
@@ -610,7 +610,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -935,8 +935,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1375,7 +1375,7 @@
         <v>14</v>
       </c>
       <c r="D31" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1668,7 +1668,7 @@
   <dimension ref="A1:D55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2012,7 +2012,7 @@
         <v>2</v>
       </c>
       <c r="D24" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
@@ -2026,7 +2026,7 @@
         <v>2</v>
       </c>
       <c r="D25" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
@@ -2458,7 +2458,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>

</xml_diff>